<commit_message>
commit mise à jour fichier
</commit_message>
<xml_diff>
--- a/CorrespondanceEntréeCDA-RessourcesFHIR.xlsx
+++ b/CorrespondanceEntréeCDA-RessourcesFHIR.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\souad\OneDrive - ANS\Bureau\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\souad\OneDrive - ANS\Bureau\correspondance FHIR CDA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43C8167F-DC38-4BEB-ADE0-212759D8FEE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{0403872C-3118-423A-9EF3-9199D9BAB8BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{6291E0F9-BC7C-469B-8D69-1F2C8DB71058}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="201">
   <si>
     <t>Donnée</t>
   </si>
@@ -2307,12 +2307,226 @@
 * location.location only Reference(FrLocationDocument)</t>
     </r>
   </si>
+  <si>
+    <t>Acte de substitution</t>
+  </si>
+  <si>
+    <t>FR-Acte-substitution</t>
+  </si>
+  <si>
+    <t>MedicationDispense.status = completed</t>
+  </si>
+  <si>
+    <t>Code de substitution</t>
+  </si>
+  <si>
+    <t>statut de la substitution</t>
+  </si>
+  <si>
+    <t>statusCode</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>utilisé directement dans la ressource FHIR</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>MedicationDispense :</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">  MedicationDispense.substitution</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">MedicationDispense.substitution.type
+* type from </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="11"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>https://smt.esante.gouv.fr/fhir/ValueSet/jdv-hl7-v3-ActSubstanceAdminSubstitutionCode-cisis</t>
+    </r>
+  </si>
+  <si>
+    <t>FR-Administration-de-derives-du-sang</t>
+  </si>
+  <si>
+    <t>Administration de dérivés du sang</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Création d'un profil fsh spécifique </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>FrObservationAdministrationDeDerivesDuSang</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> avec un Parent </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>FrSimpleObservation</t>
+    </r>
+  </si>
+  <si>
+    <t>Fixer le code : 
+* code = https://smt.esante.gouv.fr/fhir/CodeSystem/terminologie-cisis#MED-147 "Administration de dérivés du sang"</t>
+  </si>
+  <si>
+    <t>FR-Allergie-ou-hypersensibilite</t>
+  </si>
+  <si>
+    <t>Allergie ou hypersensibilité</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Type d'allergie / hypersensibilité non allergique / intolérance / idiosyncrasie</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>category</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (utilisation impossible du JDV https://smt.esante.gouv.fr/fhir/ValueSet/jdv-type-evenement-indesirable-previsible-cisis car FHIR utilise un JDV required à ce niveau : food | medication | environment | biologic
+AllergyIntoleranceCategory (Required))</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">        Dates de début et de fin</t>
+  </si>
+  <si>
+    <t>onsetPeriod.start 1..1
+onsetPeriod.end 0..1</t>
+  </si>
+  <si>
+    <t>Criticité</t>
+  </si>
+  <si>
+    <t>entryRelationship FR-Criticite</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">criticality
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>low | high | unable-to-assess
+AllergyIntoleranceCriticality (Required)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">        Statut clinique</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>clinicalStatus</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+(utilisation impossible du JDV  https://smt.esante.gouv.fr/fhir/ValueSet/jdv-hl7-allergyintolerance-clinical-cisis car FHIR utilise un JDV required à ce niveau : JDV FHIR Obligatoire : active | recurrence | relapse | inactive | remission | resolved
+Condition Clinical Status Codes (Required))</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">     entryRelationship FR-Probleme</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Réaction observée</t>
+  </si>
+  <si>
+    <t>reaction</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2335,6 +2549,14 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
       <sz val="11"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
@@ -2413,7 +2635,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
@@ -2444,6 +2666,12 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2592,8 +2820,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{F45D92C9-1F65-4435-8F72-A392D34BE380}" name="Tableau3" displayName="Tableau3" ref="A1:D79" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
-  <autoFilter ref="A1:D79" xr:uid="{F45D92C9-1F65-4435-8F72-A392D34BE380}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{F45D92C9-1F65-4435-8F72-A392D34BE380}" name="Tableau3" displayName="Tableau3" ref="A1:D92" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+  <autoFilter ref="A1:D92" xr:uid="{F45D92C9-1F65-4435-8F72-A392D34BE380}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{7A83BF85-81B2-4B14-8CA1-2F4DA1493674}" name="Donnée" dataDxfId="3"/>
     <tableColumn id="2" xr3:uid="{18E5AFA6-DE4E-4B70-AEB8-B87C88181DB2}" name="Entrée CDA" dataDxfId="2"/>
@@ -2921,10 +3149,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8FBE40E-ECAB-4FEA-B1CD-6A825B0BBB8D}">
-  <dimension ref="A1:D79"/>
+  <dimension ref="A1:D92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="D72" sqref="D72"/>
+    <sheetView tabSelected="1" topLeftCell="A77" workbookViewId="0">
+      <selection activeCell="D84" sqref="D84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3876,51 +4104,225 @@
         <v>174</v>
       </c>
     </row>
-    <row r="73" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="7"/>
-      <c r="B73" s="7"/>
-      <c r="C73" s="7"/>
-      <c r="D73" s="7"/>
-    </row>
-    <row r="74" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A74" s="7"/>
-      <c r="B74" s="7"/>
-      <c r="C74" s="7"/>
-      <c r="D74" s="7"/>
-    </row>
-    <row r="75" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A75" s="7"/>
-      <c r="B75" s="7"/>
-      <c r="C75" s="7"/>
-      <c r="D75" s="7"/>
-    </row>
-    <row r="76" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A76" s="7"/>
-      <c r="B76" s="7"/>
-      <c r="C76" s="7"/>
-      <c r="D76" s="7" t="s">
+    <row r="73" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A73" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="B73" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="C73" s="3"/>
+      <c r="D73" s="15" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" s="12" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A74" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="B74" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="C74" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="D74" s="8" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A75" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="B75" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="C75" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="D75" s="8" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A76" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="B76" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="C76" s="3"/>
+      <c r="D76" s="4" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A77" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="B77" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="C77" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="D77" s="8" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A78" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="B78" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="C78" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="D78" s="8" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A79" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="B79" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="C79" s="3"/>
+      <c r="D79" s="4"/>
+    </row>
+    <row r="80" spans="1:4" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A80" s="7" t="s">
+        <v>189</v>
+      </c>
+      <c r="B80" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="C80" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="D80" s="8" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A81" s="7" t="s">
+        <v>191</v>
+      </c>
+      <c r="B81" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="C81" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="D81" s="14" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A82" s="18" t="s">
+        <v>193</v>
+      </c>
+      <c r="B82" s="10" t="s">
+        <v>194</v>
+      </c>
+      <c r="C82" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D82" s="19" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A83" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="B83" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="C83" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D83" s="14" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" s="2" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A84" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="B84" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="C84" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D84" s="8" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A85" s="7" t="s">
+        <v>199</v>
+      </c>
+      <c r="B85" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="C85" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D85" s="14" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A86" s="7"/>
+      <c r="B86" s="7"/>
+      <c r="C86" s="7"/>
+      <c r="D86" s="7"/>
+    </row>
+    <row r="87" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A87" s="7"/>
+      <c r="B87" s="7"/>
+      <c r="C87" s="7"/>
+      <c r="D87" s="7"/>
+    </row>
+    <row r="88" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A88" s="7"/>
+      <c r="B88" s="7"/>
+      <c r="C88" s="7"/>
+      <c r="D88" s="8"/>
+    </row>
+    <row r="89" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A89" s="7"/>
+      <c r="B89" s="7"/>
+      <c r="C89" s="7"/>
+      <c r="D89" s="8" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="77" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A77" s="7"/>
-      <c r="B77" s="7"/>
-      <c r="C77" s="7"/>
-      <c r="D77" s="7" t="s">
+    <row r="90" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A90" s="7"/>
+      <c r="B90" s="7"/>
+      <c r="C90" s="7"/>
+      <c r="D90" s="8" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="78" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A78" s="7"/>
-      <c r="B78" s="7"/>
-      <c r="C78" s="7"/>
-      <c r="D78" s="7"/>
-    </row>
-    <row r="79" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A79" s="11"/>
-      <c r="B79" s="11"/>
-      <c r="C79" s="11"/>
-      <c r="D79" s="11"/>
+    <row r="91" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A91" s="7"/>
+      <c r="B91" s="7"/>
+      <c r="C91" s="7"/>
+      <c r="D91" s="8"/>
+    </row>
+    <row r="92" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A92" s="7"/>
+      <c r="B92" s="7"/>
+      <c r="C92" s="7"/>
+      <c r="D92" s="8"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>